<commit_message>
fix: update template files for improved formatting
</commit_message>
<xml_diff>
--- a/template_asn.xlsx
+++ b/template_asn.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01827A48-FDD4-4627-8F8A-A7D4DCC7DAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D048583E-5EE3-4A07-AEE3-FC285FCE1401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lembar1" sheetId="1" r:id="rId1"/>
     <sheet name="Print" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -36,9 +49,6 @@
     <t>SELONG,</t>
   </si>
   <si>
-    <t>Plt. KEPALA DINAS PERUMAHAN DAN KAWASAN PERMUKIMAN</t>
-  </si>
-  <si>
     <t>KABUPATEN LOMBOK TIMUR</t>
   </si>
   <si>
@@ -49,6 +59,9 @@
   </si>
   <si>
     <t>email : perkim@lomboktimurkab.go.id Kode Pos 83612</t>
+  </si>
+  <si>
+    <t>KEPALA DINAS PERUMAHAN DAN KAWASAN PERMUKIMAN</t>
   </si>
 </sst>
 </file>
@@ -229,6 +242,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -239,25 +271,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,8 +641,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -658,8 +671,8 @@
   </sheetPr>
   <dimension ref="A2:L41"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -676,14 +689,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="B2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -691,14 +704,14 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -706,14 +719,14 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -721,14 +734,14 @@
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="B5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -745,15 +758,15 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:12" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -766,7 +779,7 @@
       </c>
       <c r="B9" s="10">
         <f ca="1">TODAY()</f>
-        <v>45783</v>
+        <v>45874</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -789,631 +802,631 @@
       <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:12" s="14" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25">
+      <c r="A11" s="18">
         <f>lembar1!A1</f>
         <v>0</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="18">
         <f>lembar1!B1</f>
         <v>0</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="18">
         <f>lembar1!C1</f>
         <v>0</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="18">
         <f>lembar1!D1</f>
         <v>0</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="18">
         <f>lembar1!E1</f>
         <v>0</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="18">
         <f>lembar1!F1</f>
         <v>0</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="18">
         <f>lembar1!G1</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26">
+      <c r="A12" s="19">
         <f>lembar1!A2</f>
         <v>0</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="20">
         <f>lembar1!B2</f>
         <v>0</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="19">
         <f>lembar1!C2</f>
         <v>0</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="19">
         <f>lembar1!D2</f>
         <v>0</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="19">
         <f>lembar1!E2</f>
         <v>0</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="19">
         <f>lembar1!F2</f>
         <v>0</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="19">
         <f>lembar1!G2</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26">
+      <c r="A13" s="19">
         <f>lembar1!A3</f>
         <v>0</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="20">
         <f>lembar1!B3</f>
         <v>0</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="19">
         <f>lembar1!C3</f>
         <v>0</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="19">
         <f>lembar1!D3</f>
         <v>0</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="19">
         <f>lembar1!E3</f>
         <v>0</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="19">
         <f>lembar1!F3</f>
         <v>0</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="19">
         <f>lembar1!G3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="26">
+    <row r="14" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="19">
         <f>lembar1!A4</f>
         <v>0</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="20">
         <f>lembar1!B4</f>
         <v>0</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="19">
         <f>lembar1!C4</f>
         <v>0</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="19">
         <f>lembar1!D4</f>
         <v>0</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="19">
         <f>lembar1!E4</f>
         <v>0</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="19">
         <f>lembar1!F4</f>
         <v>0</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="19">
         <f>lembar1!G4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="26">
+    <row r="15" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="19">
         <f>lembar1!A5</f>
         <v>0</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="20">
         <f>lembar1!B5</f>
         <v>0</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="19">
         <f>lembar1!C5</f>
         <v>0</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="19">
         <f>lembar1!D5</f>
         <v>0</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="19">
         <f>lembar1!E5</f>
         <v>0</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="19">
         <f>lembar1!F5</f>
         <v>0</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="19">
         <f>lembar1!G5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="26">
+    <row r="16" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="19">
         <f>lembar1!A6</f>
         <v>0</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="20">
         <f>lembar1!B6</f>
         <v>0</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="19">
         <f>lembar1!C6</f>
         <v>0</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="19">
         <f>lembar1!D6</f>
         <v>0</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="19">
         <f>lembar1!E6</f>
         <v>0</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="19">
         <f>lembar1!F6</f>
         <v>0</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="19">
         <f>lembar1!G6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="26">
+    <row r="17" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
         <f>lembar1!A7</f>
         <v>0</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="20">
         <f>lembar1!B7</f>
         <v>0</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="19">
         <f>lembar1!C7</f>
         <v>0</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="19">
         <f>lembar1!D7</f>
         <v>0</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="19">
         <f>lembar1!E7</f>
         <v>0</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="19">
         <f>lembar1!F7</f>
         <v>0</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="19">
         <f>lembar1!G7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="26">
+    <row r="18" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="19">
         <f>lembar1!A8</f>
         <v>0</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="20">
         <f>lembar1!B8</f>
         <v>0</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="19">
         <f>lembar1!C8</f>
         <v>0</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="19">
         <f>lembar1!D8</f>
         <v>0</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="19">
         <f>lembar1!E8</f>
         <v>0</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="19">
         <f>lembar1!F8</f>
         <v>0</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="19">
         <f>lembar1!G8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="26">
+    <row r="19" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="19">
         <f>lembar1!A9</f>
         <v>0</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="20">
         <f>lembar1!B9</f>
         <v>0</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="19">
         <f>lembar1!C9</f>
         <v>0</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="19">
         <f>lembar1!D9</f>
         <v>0</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="19">
         <f>lembar1!E9</f>
         <v>0</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="19">
         <f>lembar1!F9</f>
         <v>0</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="19">
         <f>lembar1!G9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="26">
+    <row r="20" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="19">
         <f>lembar1!A10</f>
         <v>0</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="20">
         <f>lembar1!B10</f>
         <v>0</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="19">
         <f>lembar1!C10</f>
         <v>0</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="19">
         <f>lembar1!D10</f>
         <v>0</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="19">
         <f>lembar1!E10</f>
         <v>0</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="19">
         <f>lembar1!F10</f>
         <v>0</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="19">
         <f>lembar1!G10</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="26">
+      <c r="A21" s="19">
         <f>lembar1!A11</f>
         <v>0</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="20">
         <f>lembar1!B11</f>
         <v>0</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="19">
         <f>lembar1!C11</f>
         <v>0</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="19">
         <f>lembar1!D11</f>
         <v>0</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="19">
         <f>lembar1!E11</f>
         <v>0</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="19">
         <f>lembar1!F11</f>
         <v>0</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="19">
         <f>lembar1!G11</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="26">
+      <c r="A22" s="19">
         <f>lembar1!A12</f>
         <v>0</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="20">
         <f>lembar1!B12</f>
         <v>0</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="19">
         <f>lembar1!C12</f>
         <v>0</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="19">
         <f>lembar1!D12</f>
         <v>0</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="19">
         <f>lembar1!E12</f>
         <v>0</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="19">
         <f>lembar1!F12</f>
         <v>0</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="19">
         <f>lembar1!G12</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="26">
+      <c r="A23" s="19">
         <f>lembar1!A13</f>
         <v>0</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="20">
         <f>lembar1!B13</f>
         <v>0</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="19">
         <f>lembar1!C13</f>
         <v>0</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="19">
         <f>lembar1!D13</f>
         <v>0</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="19">
         <f>lembar1!E13</f>
         <v>0</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="19">
         <f>lembar1!F13</f>
         <v>0</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="19">
         <f>lembar1!G13</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="26">
+      <c r="A24" s="19">
         <f>lembar1!A14</f>
         <v>0</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="20">
         <f>lembar1!B14</f>
         <v>0</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="19">
         <f>lembar1!C14</f>
         <v>0</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="19">
         <f>lembar1!D14</f>
         <v>0</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="19">
         <f>lembar1!E14</f>
         <v>0</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="19">
         <f>lembar1!F14</f>
         <v>0</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="19">
         <f>lembar1!G14</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="26">
+      <c r="A25" s="19">
         <f>lembar1!A15</f>
         <v>0</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="20">
         <f>lembar1!B15</f>
         <v>0</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="19">
         <f>lembar1!C15</f>
         <v>0</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="19">
         <f>lembar1!D15</f>
         <v>0</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="19">
         <f>lembar1!E15</f>
         <v>0</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="19">
         <f>lembar1!F15</f>
         <v>0</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="19">
         <f>lembar1!G15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="26">
+    <row r="26" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="19">
         <f>lembar1!A16</f>
         <v>0</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="20">
         <f>lembar1!B16</f>
         <v>0</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="19">
         <f>lembar1!C16</f>
         <v>0</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="19">
         <f>lembar1!D16</f>
         <v>0</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="19">
         <f>lembar1!E16</f>
         <v>0</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="19">
         <f>lembar1!F16</f>
         <v>0</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="19">
         <f>lembar1!G16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="69.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="26">
+    <row r="27" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="19">
         <f>lembar1!A17</f>
         <v>0</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="20">
         <f>lembar1!B17</f>
         <v>0</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="19">
         <f>lembar1!C17</f>
         <v>0</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="19">
         <f>lembar1!D17</f>
         <v>0</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E27" s="19">
         <f>lembar1!E17</f>
         <v>0</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="19">
         <f>lembar1!F17</f>
         <v>0</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="19">
         <f>lembar1!G17</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="26">
+      <c r="A28" s="19">
         <f>lembar1!A18</f>
         <v>0</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="20">
         <f>lembar1!B18</f>
         <v>0</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="19">
         <f>lembar1!C18</f>
         <v>0</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="19">
         <f>lembar1!D18</f>
         <v>0</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="19">
         <f>lembar1!E18</f>
         <v>0</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="19">
         <f>lembar1!F18</f>
         <v>0</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="19">
         <f>lembar1!G18</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="26">
+      <c r="A29" s="19">
         <f>lembar1!A19</f>
         <v>0</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="20">
         <f>lembar1!B19</f>
         <v>0</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="19">
         <f>lembar1!C19</f>
         <v>0</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="19">
         <f>lembar1!D19</f>
         <v>0</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="19">
         <f>lembar1!E19</f>
         <v>0</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="19">
         <f>lembar1!F19</f>
         <v>0</v>
       </c>
-      <c r="G29" s="26">
+      <c r="G29" s="19">
         <f>lembar1!G19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="26">
+    <row r="30" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="19">
         <f>lembar1!A20</f>
         <v>0</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="20">
         <f>lembar1!B20</f>
         <v>0</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="19">
         <f>lembar1!C20</f>
         <v>0</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="19">
         <f>lembar1!D20</f>
         <v>0</v>
       </c>
-      <c r="E30" s="26">
+      <c r="E30" s="19">
         <f>lembar1!E20</f>
         <v>0</v>
       </c>
-      <c r="F30" s="26">
+      <c r="F30" s="19">
         <f>lembar1!F20</f>
         <v>0</v>
       </c>
-      <c r="G30" s="26">
+      <c r="G30" s="19">
         <f>lembar1!G20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="26">
+    <row r="31" spans="1:12" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="19">
         <f>lembar1!A21</f>
         <v>0</v>
       </c>
-      <c r="B31" s="27">
+      <c r="B31" s="20">
         <f>lembar1!B21</f>
         <v>0</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="19">
         <f>lembar1!C21</f>
         <v>0</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="19">
         <f>lembar1!D21</f>
         <v>0</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="19">
         <f>lembar1!E21</f>
         <v>0</v>
       </c>
-      <c r="F31" s="26">
+      <c r="F31" s="19">
         <f>lembar1!F21</f>
         <v>0</v>
       </c>
-      <c r="G31" s="26">
+      <c r="G31" s="19">
         <f>lembar1!G21</f>
         <v>0</v>
       </c>
@@ -1424,31 +1437,31 @@
       <c r="L31" s="12"/>
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="26">
+      <c r="A32" s="19">
         <f>lembar1!A22</f>
         <v>0</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="20">
         <f>lembar1!B22</f>
         <v>0</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="19">
         <f>lembar1!C22</f>
         <v>0</v>
       </c>
-      <c r="D32" s="26">
+      <c r="D32" s="19">
         <f>lembar1!D22</f>
         <v>0</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="19">
         <f>lembar1!E22</f>
         <v>0</v>
       </c>
-      <c r="F32" s="26">
+      <c r="F32" s="19">
         <f>lembar1!F22</f>
         <v>0</v>
       </c>
-      <c r="G32" s="26">
+      <c r="G32" s="19">
         <f>lembar1!G22</f>
         <v>0</v>
       </c>
@@ -1492,9 +1505,9 @@
       <c r="E35" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="28">
+      <c r="F35" s="21">
         <f ca="1">TODAY()</f>
-        <v>45783</v>
+        <v>45874</v>
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="7"/>
@@ -1509,7 +1522,7 @@
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="22" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -1525,7 +1538,7 @@
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -1554,31 +1567,31 @@
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.65">
       <c r="E41" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A8:G8"/>
     <mergeCell ref="E41:G41"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="E37:G37"/>
     <mergeCell ref="E38:G38"/>
     <mergeCell ref="E39:G39"/>
     <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A8:G8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>